<commit_message>
working on index match
</commit_message>
<xml_diff>
--- a/Excel/3 cleaning bad data/movies_indexmatch.xlsx
+++ b/Excel/3 cleaning bad data/movies_indexmatch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codebasics\Excel\3 cleaning bad data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codebasics_dataanalyst\Excel\3 cleaning bad data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DF044E-ADDF-4428-B52D-2AC79531D709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B2AB2C-DE22-4927-96EA-9C57FCB994E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="164">
   <si>
     <t>movie_id</t>
   </si>
@@ -412,9 +412,6 @@
   </si>
   <si>
     <t>Government of West Bengal</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>K.G.F: Chapter 2</t>
@@ -812,10 +809,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:G41" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:G41" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}"/>
-  <tableColumns count="7">
-    <tableColumn id="9" xr3:uid="{57CD20B6-CF66-4BAE-94B1-97E7C8A9F0F2}" name="Column1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:F41" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:F41" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D1A9B0F4-FC15-4DC9-80C7-7EBF56996521}" name="movie_id"/>
     <tableColumn id="10" xr3:uid="{58636DC6-FB58-4553-A81E-9A89F0ACE12A}" name="Column2"/>
     <tableColumn id="2" xr3:uid="{7A82C7E9-BE81-4BFD-9DE1-91C9F01BD827}" name="budget"/>
@@ -1159,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1194,7 +1190,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1233,7 +1229,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1272,7 +1268,7 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1311,7 +1307,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1350,7 +1346,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1389,7 +1385,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1428,7 +1424,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1467,7 +1463,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1506,7 +1502,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1545,7 +1541,7 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1584,7 +1580,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1623,7 +1619,7 @@
         <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1662,7 +1658,7 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1701,7 +1697,7 @@
         <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1740,7 +1736,7 @@
         <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1779,7 +1775,7 @@
         <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1818,7 +1814,7 @@
         <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1857,7 +1853,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1896,7 +1892,7 @@
         <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1935,7 +1931,7 @@
         <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1974,7 +1970,7 @@
         <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -2013,7 +2009,7 @@
         <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -2052,7 +2048,7 @@
         <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -2091,7 +2087,7 @@
         <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -2130,7 +2126,7 @@
         <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -2169,7 +2165,7 @@
         <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -2208,7 +2204,7 @@
         <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -2247,7 +2243,7 @@
         <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -2286,7 +2282,7 @@
         <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -2325,7 +2321,7 @@
         <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -2364,7 +2360,7 @@
         <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -2403,7 +2399,7 @@
         <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -2442,7 +2438,7 @@
         <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -2481,7 +2477,7 @@
         <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -2520,7 +2516,7 @@
         <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -2559,7 +2555,7 @@
         <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -2598,7 +2594,7 @@
         <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -2637,7 +2633,7 @@
         <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -2676,7 +2672,7 @@
         <v>140</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -2729,719 +2725,715 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF951C0-D968-407B-BACE-9EC26BF67B79}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>12.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>954.8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="C4">
+        <v>165</v>
+      </c>
+      <c r="D4">
+        <v>644.79999999999995</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>180</v>
+      </c>
+      <c r="D5">
+        <v>854</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <v>250</v>
+      </c>
+      <c r="D6">
+        <v>670</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>107</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>550</v>
+      </c>
+      <c r="D8">
+        <v>4000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>109</v>
+      </c>
+      <c r="C9">
+        <v>390</v>
+      </c>
+      <c r="D9">
+        <v>1360</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="C10">
+        <v>1.4</v>
+      </c>
+      <c r="D10">
+        <v>3.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>111</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>73.3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>113</v>
+      </c>
+      <c r="C12">
+        <v>165</v>
+      </c>
+      <c r="D12">
+        <v>701.8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>114</v>
+      </c>
+      <c r="C13">
+        <v>205</v>
+      </c>
+      <c r="D13">
+        <v>365.3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>115</v>
+      </c>
+      <c r="C14">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>116</v>
+      </c>
+      <c r="C15">
+        <v>103</v>
+      </c>
+      <c r="D15">
+        <v>460.5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>117</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>2202</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>3.18</v>
+      </c>
+      <c r="D17">
+        <v>3.3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>119</v>
+      </c>
+      <c r="C18">
+        <v>237</v>
+      </c>
+      <c r="D18">
+        <v>2847</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>120</v>
+      </c>
+      <c r="C19">
+        <v>7.2</v>
+      </c>
+      <c r="D19">
+        <v>291</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>121</v>
+      </c>
+      <c r="C20">
+        <v>185</v>
+      </c>
+      <c r="D20">
+        <v>1006</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>122</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>322.2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>123</v>
+      </c>
+      <c r="C22">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <v>1046</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>124</v>
+      </c>
+      <c r="C23">
+        <v>15.5</v>
+      </c>
+      <c r="D23">
+        <v>263.10000000000002</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>125</v>
+      </c>
+      <c r="C24">
+        <v>400</v>
+      </c>
+      <c r="D24">
+        <v>2798</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>126</v>
+      </c>
+      <c r="C25">
+        <v>400</v>
+      </c>
+      <c r="D25">
+        <v>2048</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>127</v>
+      </c>
+      <c r="C26">
+        <v>70</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>128</v>
+      </c>
+      <c r="C27">
+        <v>120</v>
+      </c>
+      <c r="D27">
+        <v>1350</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>129</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>410</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>130</v>
+      </c>
+      <c r="C29">
+        <v>850</v>
+      </c>
+      <c r="D29">
+        <v>8540</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>131</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>5.9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>132</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3.6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>133</v>
+      </c>
+      <c r="C32">
+        <v>5.5</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>134</v>
+      </c>
+      <c r="C33">
+        <v>1.8</v>
+      </c>
+      <c r="D33">
+        <v>6.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>135</v>
+      </c>
+      <c r="C34">
+        <v>250</v>
+      </c>
+      <c r="D34">
+        <v>3409</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>136</v>
+      </c>
+      <c r="C35">
+        <v>900</v>
+      </c>
+      <c r="D35">
+        <v>11690</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>137</v>
+      </c>
+      <c r="C36">
+        <v>216.7</v>
+      </c>
+      <c r="D36">
+        <v>370.6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>138</v>
+      </c>
+      <c r="C37">
+        <v>177</v>
+      </c>
+      <c r="D37">
+        <v>714.4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>139</v>
+      </c>
+      <c r="C38">
+        <v>1.8</v>
+      </c>
+      <c r="D38">
+        <v>3.1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>140</v>
+      </c>
+      <c r="C39">
+        <v>500</v>
+      </c>
+      <c r="D39">
+        <v>950</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>406</v>
+      </c>
+      <c r="C40">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>101</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>12.5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D40">
+        <v>350</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>102</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="E3">
-        <v>954.8</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>412</v>
+      </c>
+      <c r="C41">
+        <v>160</v>
+      </c>
+      <c r="D41">
+        <v>836.8</v>
+      </c>
+      <c r="E41" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>103</v>
-      </c>
-      <c r="D4">
-        <v>165</v>
-      </c>
-      <c r="E4">
-        <v>644.79999999999995</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>104</v>
-      </c>
-      <c r="D5">
-        <v>180</v>
-      </c>
-      <c r="E5">
-        <v>854</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>105</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-      <c r="E6">
-        <v>670</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>107</v>
-      </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-      <c r="E7">
-        <v>2000</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>108</v>
-      </c>
-      <c r="D8">
-        <v>550</v>
-      </c>
-      <c r="E8">
-        <v>4000</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>109</v>
-      </c>
-      <c r="D9">
-        <v>390</v>
-      </c>
-      <c r="E9">
-        <v>1360</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>110</v>
-      </c>
-      <c r="D10">
-        <v>1.4</v>
-      </c>
-      <c r="E10">
-        <v>3.5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>111</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>73.3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>113</v>
-      </c>
-      <c r="D12">
-        <v>165</v>
-      </c>
-      <c r="E12">
-        <v>701.8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>114</v>
-      </c>
-      <c r="D13">
-        <v>205</v>
-      </c>
-      <c r="E13">
-        <v>365.3</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>115</v>
-      </c>
-      <c r="D14">
-        <v>55</v>
-      </c>
-      <c r="E14">
-        <v>307.10000000000002</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>116</v>
-      </c>
-      <c r="D15">
-        <v>103</v>
-      </c>
-      <c r="E15">
-        <v>460.5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>117</v>
-      </c>
-      <c r="D16">
-        <v>200</v>
-      </c>
-      <c r="E16">
-        <v>2202</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>118</v>
-      </c>
-      <c r="D17">
-        <v>3.18</v>
-      </c>
-      <c r="E17">
-        <v>3.3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>119</v>
-      </c>
-      <c r="D18">
-        <v>237</v>
-      </c>
-      <c r="E18">
-        <v>2847</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>120</v>
-      </c>
-      <c r="D19">
-        <v>7.2</v>
-      </c>
-      <c r="E19">
-        <v>291</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>121</v>
-      </c>
-      <c r="D20">
-        <v>185</v>
-      </c>
-      <c r="E20">
-        <v>1006</v>
-      </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>122</v>
-      </c>
-      <c r="D21">
-        <v>22</v>
-      </c>
-      <c r="E21">
-        <v>322.2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>123</v>
-      </c>
-      <c r="D22">
-        <v>63</v>
-      </c>
-      <c r="E22">
-        <v>1046</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>124</v>
-      </c>
-      <c r="D23">
-        <v>15.5</v>
-      </c>
-      <c r="E23">
-        <v>263.10000000000002</v>
-      </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>125</v>
-      </c>
-      <c r="D24">
-        <v>400</v>
-      </c>
-      <c r="E24">
-        <v>2798</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>126</v>
-      </c>
-      <c r="D25">
-        <v>400</v>
-      </c>
-      <c r="E25">
-        <v>2048</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>127</v>
-      </c>
-      <c r="D26">
-        <v>70</v>
-      </c>
-      <c r="E26">
-        <v>100</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>128</v>
-      </c>
-      <c r="D27">
-        <v>120</v>
-      </c>
-      <c r="E27">
-        <v>1350</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28">
-        <v>129</v>
-      </c>
-      <c r="D28">
-        <v>100</v>
-      </c>
-      <c r="E28">
-        <v>410</v>
-      </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>130</v>
-      </c>
-      <c r="D29">
-        <v>850</v>
-      </c>
-      <c r="E29">
-        <v>8540</v>
-      </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>131</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>5.9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>132</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <v>3.6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>133</v>
-      </c>
-      <c r="D32">
-        <v>5.5</v>
-      </c>
-      <c r="E32">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>134</v>
-      </c>
-      <c r="D33">
-        <v>1.8</v>
-      </c>
-      <c r="E33">
-        <v>6.5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>135</v>
-      </c>
-      <c r="D34">
-        <v>250</v>
-      </c>
-      <c r="E34">
-        <v>3409</v>
-      </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>136</v>
-      </c>
-      <c r="D35">
-        <v>900</v>
-      </c>
-      <c r="E35">
-        <v>11690</v>
-      </c>
-      <c r="F35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>137</v>
-      </c>
-      <c r="D36">
-        <v>216.7</v>
-      </c>
-      <c r="E36">
-        <v>370.6</v>
-      </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <v>138</v>
-      </c>
-      <c r="D37">
-        <v>177</v>
-      </c>
-      <c r="E37">
-        <v>714.4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <v>139</v>
-      </c>
-      <c r="D38">
-        <v>1.8</v>
-      </c>
-      <c r="E38">
-        <v>3.1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39">
-        <v>140</v>
-      </c>
-      <c r="D39">
-        <v>500</v>
-      </c>
-      <c r="E39">
-        <v>950</v>
-      </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>406</v>
-      </c>
-      <c r="D40">
-        <v>30</v>
-      </c>
-      <c r="E40">
-        <v>350</v>
-      </c>
-      <c r="F40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <v>412</v>
-      </c>
-      <c r="D41">
-        <v>160</v>
-      </c>
-      <c r="E41">
-        <v>836.8</v>
-      </c>
       <c r="F41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5050,10 +5042,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226EBB25-744C-45BE-8F92-9A418CFCADCB}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="226" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="226" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5064,15 +5056,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -5084,7 +5076,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -5096,7 +5088,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4">
         <v>13</v>
@@ -5104,7 +5096,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -5117,7 +5109,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6">
         <f>MATCH("revenue", Financials[#Headers],0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -5133,6 +5125,22 @@
       <c r="D8">
         <f>MATCH("dosa",food[[#All],[item]],0)</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f>INDEX(food[],3,2)</f>
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <f>MATCH("burger",food[item],0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f>INDEX(Financials[],2,3)</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5144,6 +5152,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
+    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100686C0266E115364AA9B96DE5BECF7DB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c921848065db5a49d1de2391ec81580e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="631564f6-0349-4cc5-b00d-7cf3ba42f824" xmlns:ns3="46297aa2-77d1-4586-9726-07d56a535ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff9dd1b7eff9d7fccc1b7fb333026bb0" ns2:_="" ns3:_="">
     <xsd:import namespace="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
@@ -5372,35 +5408,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
-    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
+    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02BA008F-2FD2-4901-8027-A024DA31C6C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5417,23 +5444,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
-    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>